<commit_message>
Added methods to reflection class
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData/TestCases.xlsx
+++ b/src/main/resources/TestData/TestCases.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="25">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -25,6 +25,9 @@
     <t>Description</t>
   </si>
   <si>
+    <t>Identifier</t>
+  </si>
+  <si>
     <t>InputLocator</t>
   </si>
   <si>
@@ -41,6 +44,9 @@
   </si>
   <si>
     <t>Verify Whether User is able to login to TCI Dev</t>
+  </si>
+  <si>
+    <t>xpath</t>
   </si>
   <si>
     <t xml:space="preserve">http://tcidev-integration.sandbox.cloud.tibco.com
@@ -65,7 +71,7 @@
     <t>gkchaitu277@dispostable.com</t>
   </si>
   <si>
-    <t>clearandenter</t>
+    <t>enterText</t>
   </si>
   <si>
     <t>//button[@id='next']</t>
@@ -146,8 +152,8 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="3" max="3" width="52.71"/>
-    <col customWidth="1" min="4" max="4" width="29.71"/>
-    <col customWidth="1" min="5" max="5" width="19.0"/>
+    <col customWidth="1" min="4" max="4" width="13.57"/>
+    <col customWidth="1" min="5" max="6" width="19.0"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -178,6 +184,9 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1">
@@ -187,16 +196,19 @@
         <v>1.0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="G2" s="2" t="s">
         <v>12</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="3">
@@ -207,16 +219,19 @@
         <v>2.0</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="4">
@@ -227,19 +242,22 @@
         <v>3.0</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="5">
@@ -250,16 +268,17 @@
         <v>4.0</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="6">
@@ -270,19 +289,20 @@
         <v>5.0</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>12</v>
+      <c r="J6" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="7">
@@ -293,16 +313,17 @@
         <v>6.0</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="8">
@@ -313,18 +334,18 @@
         <v>7.0</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="F2"/>
+    <hyperlink r:id="rId1" ref="G2"/>
   </hyperlinks>
   <drawing r:id="rId2"/>
 </worksheet>

</xml_diff>

<commit_message>
Added methods to Identifiers class
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData/TestCases.xlsx
+++ b/src/main/resources/TestData/TestCases.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="26">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -37,16 +37,16 @@
     <t>Action</t>
   </si>
   <si>
+    <t>Browser</t>
+  </si>
+  <si>
+    <t>OS</t>
+  </si>
+  <si>
     <t>Comments</t>
   </si>
   <si>
-    <t>Browser</t>
-  </si>
-  <si>
     <t>Verify Whether User is able to login to TCI Dev</t>
-  </si>
-  <si>
-    <t>xpath</t>
   </si>
   <si>
     <t xml:space="preserve">http://tcidev-integration.sandbox.cloud.tibco.com
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t>chrome</t>
+  </si>
+  <si>
+    <t>xpath</t>
   </si>
   <si>
     <t>//button[@id='login']</t>
@@ -187,6 +190,9 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1">
@@ -196,9 +202,6 @@
         <v>1.0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G2" s="2" t="s">
@@ -207,7 +210,7 @@
       <c r="H2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>14</v>
       </c>
     </row>
@@ -219,18 +222,18 @@
         <v>2.0</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>14</v>
       </c>
     </row>
@@ -242,21 +245,21 @@
         <v>3.0</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="J4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>14</v>
       </c>
     </row>
@@ -268,16 +271,18 @@
         <v>4.0</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="1"/>
+        <v>11</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="F5" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>14</v>
       </c>
     </row>
@@ -289,19 +294,21 @@
         <v>5.0</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="1"/>
+        <v>11</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="F6" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="J6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I6" s="1" t="s">
         <v>14</v>
       </c>
     </row>
@@ -313,16 +320,18 @@
         <v>6.0</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="1"/>
+        <v>11</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="F7" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I7" s="1" t="s">
         <v>14</v>
       </c>
     </row>
@@ -334,12 +343,12 @@
         <v>7.0</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I8" s="1" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
CleanedUpComments and started implementing multiple testcases
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData/TestCases.xlsx
+++ b/src/main/resources/TestData/TestCases.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="27">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t>Verify Whether User is able to login to TCI Dev</t>
+  </si>
+  <si>
+    <t>chrome</t>
   </si>
   <si>
     <t xml:space="preserve">http://tcidev-integration.sandbox.cloud.tibco.com
@@ -56,9 +59,6 @@
     <t>openurl</t>
   </si>
   <si>
-    <t>chrome</t>
-  </si>
-  <si>
     <t>xpath</t>
   </si>
   <si>
@@ -90,6 +90,9 @@
   </si>
   <si>
     <t>closebrowser</t>
+  </si>
+  <si>
+    <t>Verify Whether User is able to login to TCI Dev-2</t>
   </si>
 </sst>
 </file>
@@ -204,14 +207,10 @@
       <c r="C2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
       <c r="I2" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3">
@@ -219,22 +218,19 @@
         <v>1.0</v>
       </c>
       <c r="B3" s="1">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>16</v>
+      <c r="G3" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4">
@@ -242,7 +238,7 @@
         <v>1.0</v>
       </c>
       <c r="B4" s="1">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>11</v>
@@ -251,16 +247,13 @@
         <v>15</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5">
@@ -268,7 +261,7 @@
         <v>1.0</v>
       </c>
       <c r="B5" s="1">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>11</v>
@@ -277,13 +270,16 @@
         <v>15</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6">
@@ -291,7 +287,7 @@
         <v>1.0</v>
       </c>
       <c r="B6" s="1">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>11</v>
@@ -300,16 +296,13 @@
         <v>15</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7">
@@ -317,7 +310,7 @@
         <v>1.0</v>
       </c>
       <c r="B7" s="1">
-        <v>6.0</v>
+        <v>5.0</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>11</v>
@@ -326,13 +319,16 @@
         <v>15</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8">
@@ -340,22 +336,220 @@
         <v>1.0</v>
       </c>
       <c r="B8" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="B9" s="1">
         <v>7.0</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H8" s="1" t="s">
+      <c r="C9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="I9" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H12" s="1" t="s">
         <v>14</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="B13" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="B14" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="B15" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="B16" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="B17" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="B18" s="1">
+        <v>7.0</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="G2"/>
+    <hyperlink r:id="rId1" ref="G3"/>
+    <hyperlink r:id="rId2" ref="G12"/>
   </hyperlinks>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
-Implemented TestCaseRowIndexesClass which enables framework to run the test cases based upon the entries from config.yml -Added debug steps to check test case numbers
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData/TestCases.xlsx
+++ b/src/main/resources/TestData/TestCases.xlsx
@@ -4,6 +4,7 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="TestCases" sheetId="1" r:id="rId3"/>
+    <sheet state="visible" name="ObjectRepository" sheetId="2" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -11,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="53">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -46,10 +47,46 @@
     <t>Comments</t>
   </si>
   <si>
+    <t>Alias</t>
+  </si>
+  <si>
+    <t>Locator</t>
+  </si>
+  <si>
+    <t>SigninButton</t>
+  </si>
+  <si>
+    <t>xpath</t>
+  </si>
+  <si>
+    <t>//button[@id='login']</t>
+  </si>
+  <si>
+    <t>EmailInput</t>
+  </si>
+  <si>
     <t>Verify Whether User is able to login to TCI Dev</t>
   </si>
   <si>
-    <t>chrome</t>
+    <t>//input[@id='email']</t>
+  </si>
+  <si>
+    <t>Next</t>
+  </si>
+  <si>
+    <t>//button[@id='next']</t>
+  </si>
+  <si>
+    <t>EmailPassword</t>
+  </si>
+  <si>
+    <t>//input[@id='password']</t>
+  </si>
+  <si>
+    <t>LoginButton</t>
+  </si>
+  <si>
+    <t>//button[@id='taLogin']</t>
   </si>
   <si>
     <t xml:space="preserve">http://tcidev-integration.sandbox.cloud.tibco.com
@@ -59,47 +96,89 @@
     <t>openurl</t>
   </si>
   <si>
-    <t>xpath</t>
-  </si>
-  <si>
-    <t>//button[@id='login']</t>
+    <t>chrome</t>
   </si>
   <si>
     <t>click</t>
   </si>
   <si>
-    <t>//input[@id='email']</t>
-  </si>
-  <si>
     <t>gkchaitu277@dispostable.com</t>
   </si>
   <si>
     <t>enterText</t>
   </si>
   <si>
-    <t>//button[@id='next']</t>
-  </si>
-  <si>
-    <t>//input[@id='password']</t>
-  </si>
-  <si>
     <t>Tibco2018</t>
   </si>
   <si>
-    <t>//button[@id='taLogin']</t>
-  </si>
-  <si>
-    <t>closebrowser</t>
-  </si>
-  <si>
-    <t>Verify Whether User is able to login to TCI Dev-2</t>
+    <t>10000</t>
+  </si>
+  <si>
+    <t>waittime</t>
+  </si>
+  <si>
+    <t>//div[@class='modal-dialog']</t>
+  </si>
+  <si>
+    <t>//span[@translate='TROPOS_WELCOME.ACCEPT']</t>
+  </si>
+  <si>
+    <t>linktext</t>
+  </si>
+  <si>
+    <t>Connections</t>
+  </si>
+  <si>
+    <t>60000</t>
+  </si>
+  <si>
+    <t>clickAndWait</t>
+  </si>
+  <si>
+    <t>//div[contains(@class,'wi-card-title-connector') and contains(text(),'Microsoft Azure ServiceBus Connector')]</t>
+  </si>
+  <si>
+    <t>//p-dialog[@id='connectionListModal']/div/div[2]</t>
+  </si>
+  <si>
+    <t>//input[@id='name']</t>
+  </si>
+  <si>
+    <t>AzureServiceBusConnection</t>
+  </si>
+  <si>
+    <t>//input[@id='description']</t>
+  </si>
+  <si>
+    <t>AzureServiceBusConnection-Automation</t>
+  </si>
+  <si>
+    <t>//input[@id='resourceURI']</t>
+  </si>
+  <si>
+    <t>ServicebusQA001</t>
+  </si>
+  <si>
+    <t>//input[@id='authorizationRuleName']</t>
+  </si>
+  <si>
+    <t>AuthRule</t>
+  </si>
+  <si>
+    <t>//input[@id='primarysecondaryKey']</t>
+  </si>
+  <si>
+    <t>eFxVfMG/8ssXCmm9BQFuEymrVnYpFvJWTxkr0nuXPQw=</t>
+  </si>
+  <si>
+    <t>(//button[@type='button'])[8]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -109,6 +188,11 @@
     <font>
       <u/>
       <color rgb="FF0000FF"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color rgb="FF000000"/>
+      <name val="'Calibri'"/>
     </font>
   </fonts>
   <fills count="2">
@@ -125,7 +209,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -133,6 +217,12 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf quotePrefix="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -144,6 +234,10 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 
@@ -159,7 +253,8 @@
   <cols>
     <col customWidth="1" min="3" max="3" width="52.71"/>
     <col customWidth="1" min="4" max="4" width="13.57"/>
-    <col customWidth="1" min="5" max="6" width="19.0"/>
+    <col customWidth="1" min="5" max="5" width="19.0"/>
+    <col customWidth="1" min="6" max="6" width="40.71"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -205,12 +300,16 @@
         <v>1.0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
+        <v>17</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="I2" s="1" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3">
@@ -218,19 +317,22 @@
         <v>1.0</v>
       </c>
       <c r="B3" s="1">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>13</v>
+        <v>17</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4">
@@ -238,22 +340,25 @@
         <v>1.0</v>
       </c>
       <c r="B4" s="1">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5">
@@ -261,25 +366,22 @@
         <v>1.0</v>
       </c>
       <c r="B5" s="1">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6">
@@ -287,22 +389,25 @@
         <v>1.0</v>
       </c>
       <c r="B6" s="1">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7">
@@ -310,25 +415,22 @@
         <v>1.0</v>
       </c>
       <c r="B7" s="1">
-        <v>5.0</v>
+        <v>6.0</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8">
@@ -336,22 +438,21 @@
         <v>1.0</v>
       </c>
       <c r="B8" s="1">
-        <v>6.0</v>
+        <v>7.0</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>24</v>
+        <v>17</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9">
@@ -359,197 +460,365 @@
         <v>1.0</v>
       </c>
       <c r="B9" s="1">
-        <v>7.0</v>
+        <v>8.0</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>11</v>
+        <v>17</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>12</v>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="B10" s="1">
+        <v>9.0</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="B11" s="1">
-        <v>1.0</v>
+        <v>10.0</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
+        <v>17</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="I11" s="1" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="B12" s="1">
-        <v>1.0</v>
+        <v>11.0</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>13</v>
+        <v>17</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="B13" s="1">
-        <v>2.0</v>
+        <v>12.0</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="G13" s="1"/>
       <c r="H13" s="1" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="B14" s="1">
-        <v>3.0</v>
+        <v>13.0</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="B15" s="1">
-        <v>4.0</v>
+        <v>14.0</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>21</v>
+        <v>44</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="B16" s="1">
-        <v>5.0</v>
+        <v>15.0</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="B17" s="1">
-        <v>6.0</v>
+        <v>16.0</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>24</v>
+        <v>48</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>49</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="B18" s="1">
-        <v>7.0</v>
+        <v>17.0</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>26</v>
+        <v>17</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>51</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>12</v>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="B19" s="1">
+        <v>18.0</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G19" s="1">
+        <v>10000.0</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="G3"/>
-    <hyperlink r:id="rId2" ref="G12"/>
+    <hyperlink r:id="rId1" ref="G2"/>
   </hyperlinks>
-  <drawing r:id="rId3"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="2" max="2" width="8.0"/>
+    <col customWidth="1" min="3" max="3" width="20.29"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
-Implemented createConnection method in keywordsActions class which enables user to create connection with just one test step
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData/TestCases.xlsx
+++ b/src/main/resources/TestData/TestCases.xlsx
@@ -12,11 +12,20 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="55">
+  <si>
+    <t>Alias</t>
+  </si>
   <si>
     <t>TestCaseID</t>
   </si>
   <si>
+    <t>Identifier</t>
+  </si>
+  <si>
+    <t>Locator</t>
+  </si>
+  <si>
     <t>TestStepNumber</t>
   </si>
   <si>
@@ -26,7 +35,7 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Identifier</t>
+    <t>SigninButton</t>
   </si>
   <si>
     <t>InputLocator</t>
@@ -35,9 +44,15 @@
     <t>InputData</t>
   </si>
   <si>
+    <t>xpath</t>
+  </si>
+  <si>
     <t>Action</t>
   </si>
   <si>
+    <t>//button[@id='login']</t>
+  </si>
+  <si>
     <t>Browser</t>
   </si>
   <si>
@@ -47,52 +62,37 @@
     <t>Comments</t>
   </si>
   <si>
-    <t>Alias</t>
-  </si>
-  <si>
-    <t>Locator</t>
-  </si>
-  <si>
-    <t>SigninButton</t>
-  </si>
-  <si>
-    <t>xpath</t>
-  </si>
-  <si>
-    <t>//button[@id='login']</t>
-  </si>
-  <si>
     <t>EmailInput</t>
   </si>
   <si>
+    <t>//input[@id='email']</t>
+  </si>
+  <si>
+    <t>Next</t>
+  </si>
+  <si>
+    <t>//button[@id='next']</t>
+  </si>
+  <si>
     <t>Verify Whether User is able to login to TCI Dev</t>
   </si>
   <si>
-    <t>//input[@id='email']</t>
-  </si>
-  <si>
-    <t>Next</t>
-  </si>
-  <si>
-    <t>//button[@id='next']</t>
-  </si>
-  <si>
     <t>EmailPassword</t>
   </si>
   <si>
     <t>//input[@id='password']</t>
-  </si>
-  <si>
-    <t>LoginButton</t>
-  </si>
-  <si>
-    <t>//button[@id='taLogin']</t>
   </si>
   <si>
     <t xml:space="preserve">http://tcidev-integration.sandbox.cloud.tibco.com
 </t>
   </si>
   <si>
+    <t>LoginButton</t>
+  </si>
+  <si>
+    <t>//button[@id='taLogin']</t>
+  </si>
+  <si>
     <t>openurl</t>
   </si>
   <si>
@@ -121,6 +121,12 @@
   </si>
   <si>
     <t>//span[@translate='TROPOS_WELCOME.ACCEPT']</t>
+  </si>
+  <si>
+    <t>Connector:'Microsoft Azure Storage Connector',name:'AzureStorageConnector',description:'description',accountName:'tibcodevstoragev2',connectionType:'Generate SAS',expiryDate:'2018-12-20T21:55:07Z',accessKey:'JUMuqVI6MO36YpT6zCxxAqj+3md8t2uu1X70gIbxNun1pmdWElOaeYkZog8DjJ/JIN04DuFTU0cR22hfcNQa5g=='</t>
+  </si>
+  <si>
+    <t>createConnection</t>
   </si>
   <si>
     <t>linktext</t>
@@ -251,7 +257,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="3" max="3" width="52.71"/>
+    <col customWidth="1" min="3" max="3" width="41.71"/>
     <col customWidth="1" min="4" max="4" width="13.57"/>
     <col customWidth="1" min="5" max="5" width="19.0"/>
     <col customWidth="1" min="6" max="6" width="40.71"/>
@@ -259,37 +265,37 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2">
@@ -300,10 +306,10 @@
         <v>1.0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>26</v>
@@ -320,13 +326,13 @@
         <v>2.0</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>28</v>
@@ -343,13 +349,13 @@
         <v>3.0</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>29</v>
@@ -369,13 +375,13 @@
         <v>4.0</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>28</v>
@@ -392,10 +398,10 @@
         <v>5.0</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>22</v>
@@ -418,13 +424,13 @@
         <v>6.0</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>28</v>
@@ -441,7 +447,7 @@
         <v>7.0</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -463,10 +469,10 @@
         <v>8.0</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>34</v>
@@ -486,10 +492,10 @@
         <v>9.0</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>35</v>
@@ -509,64 +515,56 @@
         <v>10.0</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="H11" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="I11" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" s="1">
+        <v>10.0</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="I11" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="B12" s="1">
+      <c r="G12" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" s="1">
         <v>11.0</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="B13" s="1">
-        <v>12.0</v>
-      </c>
       <c r="C13" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G13" s="1"/>
+        <v>42</v>
+      </c>
       <c r="H13" s="1" t="s">
         <v>28</v>
       </c>
@@ -575,43 +573,35 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="1">
-        <v>1.0</v>
-      </c>
       <c r="B14" s="1">
+        <v>12.0</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" s="1">
         <v>13.0</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="B15" s="1">
-        <v>14.0</v>
-      </c>
       <c r="C15" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>44</v>
@@ -627,17 +617,14 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="1">
-        <v>1.0</v>
-      </c>
       <c r="B16" s="1">
-        <v>15.0</v>
+        <v>14.0</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>46</v>
@@ -653,22 +640,19 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="1">
-        <v>1.0</v>
-      </c>
       <c r="B17" s="1">
-        <v>16.0</v>
+        <v>15.0</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="G17" s="4" t="s">
+      <c r="G17" s="1" t="s">
         <v>49</v>
       </c>
       <c r="H17" s="1" t="s">
@@ -679,22 +663,19 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="1">
-        <v>1.0</v>
-      </c>
       <c r="B18" s="1">
-        <v>17.0</v>
+        <v>16.0</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="G18" s="1" t="s">
+      <c r="G18" s="4" t="s">
         <v>51</v>
       </c>
       <c r="H18" s="1" t="s">
@@ -705,28 +686,48 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="1">
-        <v>1.0</v>
-      </c>
       <c r="B19" s="1">
-        <v>18.0</v>
+        <v>17.0</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="G19" s="1">
+      <c r="G19" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="B20" s="1">
+        <v>18.0</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G20" s="1">
         <v>10000.0</v>
       </c>
-      <c r="H19" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I19" s="1" t="s">
+      <c r="H20" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I20" s="1" t="s">
         <v>27</v>
       </c>
     </row>
@@ -754,24 +755,24 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3">
@@ -779,21 +780,21 @@
         <v>16</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="5">
@@ -801,7 +802,7 @@
         <v>21</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>22</v>
@@ -809,13 +810,13 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
-Implemented parameterization with TestNG
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData/TestCases.xlsx
+++ b/src/main/resources/TestData/TestCases.xlsx
@@ -12,11 +12,53 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="38">
+  <si>
+    <t>Alias</t>
+  </si>
   <si>
     <t>TestCaseID</t>
   </si>
   <si>
+    <t>Identifier</t>
+  </si>
+  <si>
+    <t>Locator</t>
+  </si>
+  <si>
+    <t>SigninButton</t>
+  </si>
+  <si>
+    <t>xpath</t>
+  </si>
+  <si>
+    <t>//button[@id='login']</t>
+  </si>
+  <si>
+    <t>EmailInput</t>
+  </si>
+  <si>
+    <t>//input[@id='email']</t>
+  </si>
+  <si>
+    <t>Next</t>
+  </si>
+  <si>
+    <t>//button[@id='next']</t>
+  </si>
+  <si>
+    <t>EmailPassword</t>
+  </si>
+  <si>
+    <t>//input[@id='password']</t>
+  </si>
+  <si>
+    <t>LoginButton</t>
+  </si>
+  <si>
+    <t>//button[@id='taLogin']</t>
+  </si>
+  <si>
     <t>TestStepNumber</t>
   </si>
   <si>
@@ -24,48 +66,6 @@
   </si>
   <si>
     <t>Description</t>
-  </si>
-  <si>
-    <t>Alias</t>
-  </si>
-  <si>
-    <t>Identifier</t>
-  </si>
-  <si>
-    <t>Locator</t>
-  </si>
-  <si>
-    <t>SigninButton</t>
-  </si>
-  <si>
-    <t>xpath</t>
-  </si>
-  <si>
-    <t>//button[@id='login']</t>
-  </si>
-  <si>
-    <t>EmailInput</t>
-  </si>
-  <si>
-    <t>//input[@id='email']</t>
-  </si>
-  <si>
-    <t>Next</t>
-  </si>
-  <si>
-    <t>//button[@id='next']</t>
-  </si>
-  <si>
-    <t>EmailPassword</t>
-  </si>
-  <si>
-    <t>//input[@id='password']</t>
-  </si>
-  <si>
-    <t>LoginButton</t>
-  </si>
-  <si>
-    <t>//button[@id='taLogin']</t>
   </si>
   <si>
     <t>InputLocator</t>
@@ -127,64 +127,13 @@
   </si>
   <si>
     <t>createConnection</t>
-  </si>
-  <si>
-    <t>linktext</t>
-  </si>
-  <si>
-    <t>Connections</t>
-  </si>
-  <si>
-    <t>60000</t>
-  </si>
-  <si>
-    <t>clickAndWait</t>
-  </si>
-  <si>
-    <t>//div[contains(@class,'wi-card-title-connector') and contains(text(),'Microsoft Azure ServiceBus Connector')]</t>
-  </si>
-  <si>
-    <t>//p-dialog[@id='connectionListModal']/div/div[2]</t>
-  </si>
-  <si>
-    <t>//input[@id='name']</t>
-  </si>
-  <si>
-    <t>AzureServiceBusConnection</t>
-  </si>
-  <si>
-    <t>//input[@id='description']</t>
-  </si>
-  <si>
-    <t>AzureServiceBusConnection-Automation</t>
-  </si>
-  <si>
-    <t>//input[@id='resourceURI']</t>
-  </si>
-  <si>
-    <t>ServicebusQA001</t>
-  </si>
-  <si>
-    <t>//input[@id='authorizationRuleName']</t>
-  </si>
-  <si>
-    <t>AuthRule</t>
-  </si>
-  <si>
-    <t>//input[@id='primarysecondaryKey']</t>
-  </si>
-  <si>
-    <t>eFxVfMG/8ssXCmm9BQFuEymrVnYpFvJWTxkr0nuXPQw=</t>
-  </si>
-  <si>
-    <t>(//button[@type='button'])[8]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -194,11 +143,6 @@
     <font>
       <u/>
       <color rgb="FF0000FF"/>
-    </font>
-    <font>
-      <sz val="11.0"/>
-      <color rgb="FF000000"/>
-      <name val="'Calibri'"/>
     </font>
   </fonts>
   <fills count="2">
@@ -215,7 +159,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -226,9 +170,6 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf quotePrefix="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -265,19 +206,19 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>5</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>18</v>
@@ -329,10 +270,10 @@
         <v>24</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>28</v>
@@ -352,10 +293,10 @@
         <v>24</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>29</v>
@@ -378,10 +319,10 @@
         <v>24</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>28</v>
@@ -401,10 +342,10 @@
         <v>24</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>31</v>
@@ -427,10 +368,10 @@
         <v>24</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>28</v>
@@ -472,7 +413,7 @@
         <v>24</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>34</v>
@@ -495,7 +436,7 @@
         <v>24</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>35</v>
@@ -529,85 +470,67 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12">
-      <c r="B12" s="1">
-        <v>10.0</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
     <row r="13">
+      <c r="A13" s="1">
+        <v>2.0</v>
+      </c>
       <c r="B13" s="1">
-        <v>11.0</v>
+        <v>1.0</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="G13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="B14" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="B15" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F15" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F13" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="B14" s="1">
-        <v>12.0</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="B15" s="1">
-        <v>13.0</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="G15" s="1" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>30</v>
@@ -617,43 +540,46 @@
       </c>
     </row>
     <row r="16">
+      <c r="A16" s="1">
+        <v>2.0</v>
+      </c>
       <c r="B16" s="1">
-        <v>14.0</v>
+        <v>4.0</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>47</v>
+        <v>10</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="17">
+      <c r="A17" s="1">
+        <v>2.0</v>
+      </c>
       <c r="B17" s="1">
-        <v>15.0</v>
+        <v>5.0</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>48</v>
+        <v>12</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>30</v>
@@ -663,79 +589,356 @@
       </c>
     </row>
     <row r="18">
+      <c r="A18" s="1">
+        <v>2.0</v>
+      </c>
       <c r="B18" s="1">
-        <v>16.0</v>
+        <v>6.0</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>24</v>
       </c>
       <c r="E18" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="B19" s="1">
+        <v>7.0</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="B20" s="1">
+        <v>8.0</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="B21" s="1">
+        <v>9.0</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="B22" s="1">
+        <v>10.0</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="B24" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="B25" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="B26" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F26" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F18" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="H18" s="1" t="s">
+      <c r="G26" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H26" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="I18" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="B19" s="1">
-        <v>17.0</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="H19" s="1" t="s">
+      <c r="I26" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="B27" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="B28" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H28" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="I19" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="B20" s="1">
-        <v>18.0</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G20" s="1">
-        <v>10000.0</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="I20" s="1" t="s">
+      <c r="I28" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="B29" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="B30" s="1">
+        <v>7.0</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="B31" s="1">
+        <v>8.0</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="B32" s="1">
+        <v>9.0</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="B33" s="1">
+        <v>10.0</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I33" s="1" t="s">
         <v>27</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="G2"/>
+    <hyperlink r:id="rId2" ref="G13"/>
+    <hyperlink r:id="rId3" ref="G24"/>
   </hyperlinks>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -755,68 +958,68 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>